<commit_message>
Created new features. Still waiting on data update.
</commit_message>
<xml_diff>
--- a/TN_Age.xlsx
+++ b/TN_Age.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="25">
   <si>
     <t>0-10</t>
   </si>
@@ -435,11 +435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H281"/>
+  <dimension ref="A1:H291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H287" sqref="H287:H290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5514,7 +5514,7 @@
         <v>51</v>
       </c>
       <c r="D222" s="2">
-        <f t="shared" ref="D222:D281" si="51">C222/SUMIF(A:A,A222,C:C)</f>
+        <f t="shared" ref="D222:D285" si="51">C222/SUMIF(A:A,A222,C:C)</f>
         <v>1.1005610703495899E-2</v>
       </c>
       <c r="E222" s="3">
@@ -5789,7 +5789,7 @@
         <v>1</v>
       </c>
       <c r="H232" s="3">
-        <f t="shared" ref="H232:H281" si="54">G232-SUMIFS(G:G,A:A,A232-1,B:B,B232)</f>
+        <f t="shared" ref="H232:H291" si="54">G232-SUMIFS(G:G,A:A,A232-1,B:B,B232)</f>
         <v>0</v>
       </c>
     </row>
@@ -6678,11 +6678,11 @@
         <v>1.1229946524064172E-2</v>
       </c>
       <c r="E262" s="3">
-        <f t="shared" ref="E262:E281" si="57">C262-SUMIFS(C:C,A:A,A262-1,B:B,B262)</f>
+        <f t="shared" ref="E262:E291" si="57">C262-SUMIFS(C:C,A:A,A262-1,B:B,B262)</f>
         <v>2</v>
       </c>
       <c r="F262" s="2">
-        <f t="shared" ref="F262:F281" si="58">E262/SUMIF(A:A,A262,E:E)</f>
+        <f t="shared" ref="F262:F291" si="58">E262/SUMIF(A:A,A262,E:E)</f>
         <v>6.6225165562913907E-3</v>
       </c>
       <c r="G262" s="3">
@@ -7259,6 +7259,306 @@
         <v>0</v>
       </c>
       <c r="H281" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A282" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C282" s="3">
+        <v>70</v>
+      </c>
+      <c r="D282" s="2">
+        <f t="shared" si="51"/>
+        <v>1.151505181773318E-2</v>
+      </c>
+      <c r="E282" s="3">
+        <f t="shared" si="57"/>
+        <v>2</v>
+      </c>
+      <c r="F282" s="2">
+        <f t="shared" si="58"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G282" s="3">
+        <v>1</v>
+      </c>
+      <c r="H282" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A283" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1</v>
+      </c>
+      <c r="C283" s="3">
+        <v>272</v>
+      </c>
+      <c r="D283" s="2">
+        <f t="shared" si="51"/>
+        <v>4.4744201348906068E-2</v>
+      </c>
+      <c r="E283" s="3">
+        <f t="shared" si="57"/>
+        <v>2</v>
+      </c>
+      <c r="F283" s="2">
+        <f t="shared" si="58"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G283" s="3">
+        <v>0</v>
+      </c>
+      <c r="H283" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A284" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B284" t="s">
+        <v>2</v>
+      </c>
+      <c r="C284" s="3">
+        <v>1189</v>
+      </c>
+      <c r="D284" s="2">
+        <f t="shared" si="51"/>
+        <v>0.19559138016121072</v>
+      </c>
+      <c r="E284" s="3">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="F284" s="2">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="G284" s="3">
+        <v>1</v>
+      </c>
+      <c r="H284" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A285" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B285" t="s">
+        <v>3</v>
+      </c>
+      <c r="C285" s="3">
+        <v>958</v>
+      </c>
+      <c r="D285" s="2">
+        <f t="shared" si="51"/>
+        <v>0.15759170916269125</v>
+      </c>
+      <c r="E285" s="3">
+        <f t="shared" si="57"/>
+        <v>4</v>
+      </c>
+      <c r="F285" s="2">
+        <f t="shared" si="58"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G285" s="3">
+        <v>1</v>
+      </c>
+      <c r="H285" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A286" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B286" t="s">
+        <v>4</v>
+      </c>
+      <c r="C286" s="3">
+        <v>969</v>
+      </c>
+      <c r="D286" s="2">
+        <f t="shared" ref="D286:D291" si="59">C286/SUMIF(A:A,A286,C:C)</f>
+        <v>0.15940121730547788</v>
+      </c>
+      <c r="E286" s="3">
+        <f t="shared" si="57"/>
+        <v>4</v>
+      </c>
+      <c r="F286" s="2">
+        <f t="shared" si="58"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G286" s="3">
+        <v>7</v>
+      </c>
+      <c r="H286" s="3">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A287" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B287" t="s">
+        <v>5</v>
+      </c>
+      <c r="C287" s="3">
+        <v>1076</v>
+      </c>
+      <c r="D287" s="2">
+        <f t="shared" si="59"/>
+        <v>0.1770027965125843</v>
+      </c>
+      <c r="E287" s="3">
+        <f t="shared" si="57"/>
+        <v>2</v>
+      </c>
+      <c r="F287" s="2">
+        <f t="shared" si="58"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G287" s="3">
+        <v>14</v>
+      </c>
+      <c r="H287" s="3">
+        <f t="shared" si="54"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A288" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288" s="3">
+        <v>731</v>
+      </c>
+      <c r="D288" s="2">
+        <f t="shared" si="59"/>
+        <v>0.12025004112518506</v>
+      </c>
+      <c r="E288" s="3">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="F288" s="2">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="G288" s="3">
+        <v>34</v>
+      </c>
+      <c r="H288" s="3">
+        <f t="shared" si="54"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A289" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B289" t="s">
+        <v>7</v>
+      </c>
+      <c r="C289" s="3">
+        <v>353</v>
+      </c>
+      <c r="D289" s="2">
+        <f t="shared" si="59"/>
+        <v>5.8068761309425891E-2</v>
+      </c>
+      <c r="E289" s="3">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="F289" s="2">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="G289" s="3">
+        <v>33</v>
+      </c>
+      <c r="H289" s="3">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A290" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B290" t="s">
+        <v>8</v>
+      </c>
+      <c r="C290" s="3">
+        <v>197</v>
+      </c>
+      <c r="D290" s="2">
+        <f t="shared" si="59"/>
+        <v>3.2406645829906232E-2</v>
+      </c>
+      <c r="E290" s="3">
+        <f t="shared" si="57"/>
+        <v>-2</v>
+      </c>
+      <c r="F290" s="2">
+        <f t="shared" si="58"/>
+        <v>-7.8125E-3</v>
+      </c>
+      <c r="G290" s="3">
+        <v>44</v>
+      </c>
+      <c r="H290" s="3">
+        <f t="shared" si="54"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A291" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B291" t="s">
+        <v>22</v>
+      </c>
+      <c r="C291" s="3">
+        <v>264</v>
+      </c>
+      <c r="D291" s="2">
+        <f t="shared" si="59"/>
+        <v>4.3428195426879423E-2</v>
+      </c>
+      <c r="E291" s="3">
+        <f t="shared" si="57"/>
+        <v>244</v>
+      </c>
+      <c r="F291" s="2">
+        <f t="shared" si="58"/>
+        <v>0.953125</v>
+      </c>
+      <c r="G291" s="3">
+        <v>0</v>
+      </c>
+      <c r="H291" s="3">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Data update for 5/10
</commit_message>
<xml_diff>
--- a/TN_Age.xlsx
+++ b/TN_Age.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="26">
   <si>
     <t>0-10</t>
   </si>
@@ -440,11 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I531"/>
+  <dimension ref="A1:I541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K533" sqref="K533"/>
+      <pane ySplit="1" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G532" sqref="G532:G541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16012,6 +16012,346 @@
         <v>0</v>
       </c>
     </row>
+    <row r="532" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A532" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B532" t="s">
+        <v>0</v>
+      </c>
+      <c r="C532" s="2">
+        <v>348</v>
+      </c>
+      <c r="D532" s="6">
+        <f t="shared" ref="D532:D541" si="175">C532/SUMIF(A:A,A532,C:C)</f>
+        <v>2.3223223223223222E-2</v>
+      </c>
+      <c r="E532" s="7">
+        <f t="shared" ref="E532:E541" si="176">C532-SUMIFS(C:C,A:A,A532-1,B:B,B532)</f>
+        <v>8</v>
+      </c>
+      <c r="F532" s="6">
+        <f t="shared" ref="F532:F541" si="177">E532/SUMIF(A:A,A532,E:E)</f>
+        <v>3.6866359447004608E-2</v>
+      </c>
+      <c r="G532" s="2">
+        <v>1</v>
+      </c>
+      <c r="H532" s="7">
+        <f t="shared" ref="H532:H541" si="178">G532-SUMIFS(G:G,A:A,A532-1,B:B,B532)</f>
+        <v>0</v>
+      </c>
+      <c r="I532" s="6">
+        <f t="shared" ref="I532:I541" si="179">G532/SUMIF(A:A,A532,G:G)</f>
+        <v>4.11522633744856E-3</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A533" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B533" t="s">
+        <v>1</v>
+      </c>
+      <c r="C533" s="2">
+        <v>969</v>
+      </c>
+      <c r="D533" s="6">
+        <f t="shared" si="175"/>
+        <v>6.4664664664664667E-2</v>
+      </c>
+      <c r="E533" s="7">
+        <f t="shared" si="176"/>
+        <v>27</v>
+      </c>
+      <c r="F533" s="6">
+        <f t="shared" si="177"/>
+        <v>0.12442396313364056</v>
+      </c>
+      <c r="G533" s="2">
+        <v>1</v>
+      </c>
+      <c r="H533" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I533" s="6">
+        <f t="shared" si="179"/>
+        <v>4.11522633744856E-3</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A534" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B534" t="s">
+        <v>2</v>
+      </c>
+      <c r="C534" s="2">
+        <v>2939</v>
+      </c>
+      <c r="D534" s="6">
+        <f t="shared" si="175"/>
+        <v>0.19612946279612947</v>
+      </c>
+      <c r="E534" s="7">
+        <f t="shared" si="176"/>
+        <v>34</v>
+      </c>
+      <c r="F534" s="6">
+        <f t="shared" si="177"/>
+        <v>0.15668202764976957</v>
+      </c>
+      <c r="G534" s="2">
+        <v>1</v>
+      </c>
+      <c r="H534" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I534" s="6">
+        <f t="shared" si="179"/>
+        <v>4.11522633744856E-3</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A535" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B535" t="s">
+        <v>3</v>
+      </c>
+      <c r="C535" s="2">
+        <v>2886</v>
+      </c>
+      <c r="D535" s="6">
+        <f t="shared" si="175"/>
+        <v>0.19259259259259259</v>
+      </c>
+      <c r="E535" s="7">
+        <f t="shared" si="176"/>
+        <v>47</v>
+      </c>
+      <c r="F535" s="6">
+        <f t="shared" si="177"/>
+        <v>0.21658986175115208</v>
+      </c>
+      <c r="G535" s="2">
+        <v>3</v>
+      </c>
+      <c r="H535" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I535" s="6">
+        <f t="shared" si="179"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A536" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B536" t="s">
+        <v>4</v>
+      </c>
+      <c r="C536" s="2">
+        <v>2632</v>
+      </c>
+      <c r="D536" s="6">
+        <f t="shared" si="175"/>
+        <v>0.17564230897564231</v>
+      </c>
+      <c r="E536" s="7">
+        <f t="shared" si="176"/>
+        <v>36</v>
+      </c>
+      <c r="F536" s="6">
+        <f t="shared" si="177"/>
+        <v>0.16589861751152074</v>
+      </c>
+      <c r="G536" s="2">
+        <v>9</v>
+      </c>
+      <c r="H536" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I536" s="6">
+        <f t="shared" si="179"/>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A537" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B537" t="s">
+        <v>5</v>
+      </c>
+      <c r="C537" s="2">
+        <v>2402</v>
+      </c>
+      <c r="D537" s="6">
+        <f t="shared" si="175"/>
+        <v>0.16029362696029362</v>
+      </c>
+      <c r="E537" s="7">
+        <f t="shared" si="176"/>
+        <v>25</v>
+      </c>
+      <c r="F537" s="6">
+        <f t="shared" si="177"/>
+        <v>0.1152073732718894</v>
+      </c>
+      <c r="G537" s="2">
+        <v>18</v>
+      </c>
+      <c r="H537" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I537" s="6">
+        <f t="shared" si="179"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A538" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B538" t="s">
+        <v>6</v>
+      </c>
+      <c r="C538" s="2">
+        <v>1462</v>
+      </c>
+      <c r="D538" s="6">
+        <f t="shared" si="175"/>
+        <v>9.7564230897564233E-2</v>
+      </c>
+      <c r="E538" s="7">
+        <f t="shared" si="176"/>
+        <v>16</v>
+      </c>
+      <c r="F538" s="6">
+        <f t="shared" si="177"/>
+        <v>7.3732718894009217E-2</v>
+      </c>
+      <c r="G538" s="2">
+        <v>53</v>
+      </c>
+      <c r="H538" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I538" s="6">
+        <f t="shared" si="179"/>
+        <v>0.21810699588477367</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A539" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B539" t="s">
+        <v>7</v>
+      </c>
+      <c r="C539" s="2">
+        <v>706</v>
+      </c>
+      <c r="D539" s="6">
+        <f t="shared" si="175"/>
+        <v>4.7113780447113777E-2</v>
+      </c>
+      <c r="E539" s="7">
+        <f t="shared" si="176"/>
+        <v>8</v>
+      </c>
+      <c r="F539" s="6">
+        <f t="shared" si="177"/>
+        <v>3.6866359447004608E-2</v>
+      </c>
+      <c r="G539" s="2">
+        <v>72</v>
+      </c>
+      <c r="H539" s="7">
+        <f t="shared" si="178"/>
+        <v>1</v>
+      </c>
+      <c r="I539" s="6">
+        <f t="shared" si="179"/>
+        <v>0.29629629629629628</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A540" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B540" t="s">
+        <v>25</v>
+      </c>
+      <c r="C540" s="2">
+        <v>445</v>
+      </c>
+      <c r="D540" s="6">
+        <f t="shared" si="175"/>
+        <v>2.9696363029696363E-2</v>
+      </c>
+      <c r="E540" s="7">
+        <f t="shared" si="176"/>
+        <v>4</v>
+      </c>
+      <c r="F540" s="6">
+        <f t="shared" si="177"/>
+        <v>1.8433179723502304E-2</v>
+      </c>
+      <c r="G540" s="2">
+        <v>85</v>
+      </c>
+      <c r="H540" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I540" s="6">
+        <f t="shared" si="179"/>
+        <v>0.34979423868312759</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A541" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B541" t="s">
+        <v>21</v>
+      </c>
+      <c r="C541" s="2">
+        <v>196</v>
+      </c>
+      <c r="D541" s="6">
+        <f t="shared" si="175"/>
+        <v>1.3079746413079747E-2</v>
+      </c>
+      <c r="E541" s="7">
+        <f t="shared" si="176"/>
+        <v>12</v>
+      </c>
+      <c r="F541" s="6">
+        <f t="shared" si="177"/>
+        <v>5.5299539170506916E-2</v>
+      </c>
+      <c r="G541" s="2">
+        <v>0</v>
+      </c>
+      <c r="H541" s="7">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I541" s="6">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>